<commit_message>
added comments for genyaml.py
</commit_message>
<xml_diff>
--- a/CIS-Audit-Reqs-Windows2019Server.xlsx
+++ b/CIS-Audit-Reqs-Windows2019Server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iantibble/PycharmProjects/auditpol-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5404EF76-307B-0749-A93F-F9833116EB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1A7E42-735D-F245-B8BE-B1D54DB0C7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32120" yWindow="4980" windowWidth="32740" windowHeight="23620" xr2:uid="{6829E842-9E69-7449-BDE6-C9133EB1D88E}"/>
   </bookViews>
@@ -1339,9 +1339,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE63132-7FEC-EC48-8854-0EBDD19B9D3B}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2009,11 +2009,11 @@
       <c r="F30" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>51</v>
       </c>
@@ -2032,7 +2032,7 @@
       <c r="F31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="5" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>